<commit_message>
Updating test.xls and pom.xml
</commit_message>
<xml_diff>
--- a/SugarCrm_Project/Test.xlsx
+++ b/SugarCrm_Project/Test.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
-  <workbookPr defaultThemeVersion="124226" filterPrivacy="1"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26327"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF804710-FD80-4D72-849A-6CC9B50BD1B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView windowHeight="8010" windowWidth="14805" xWindow="240" yWindow="105"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" r:id="rId1" sheetId="1"/>
-    <sheet name="Sheet2" r:id="rId2" sheetId="2"/>
-    <sheet name="Test" r:id="rId3" sheetId="3"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Test" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="9">
   <si>
     <t>I am Pramod</t>
   </si>
@@ -36,20 +37,19 @@
     <t>pass</t>
   </si>
   <si>
-    <t>123rtt6</t>
-  </si>
-  <si>
     <t>Pass</t>
   </si>
   <si>
     <t>passs</t>
+  </si>
+  <si>
+    <t>Admin</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -92,28 +92,28 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+  <cellXfs count="3">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleMedium9" defaultTableStyle="TableStyleMedium2"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -124,10 +124,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -162,7 +162,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -195,9 +195,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -230,6 +247,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -285,7 +319,7 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="9525">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="95000"/>
@@ -294,13 +328,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="25400">
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="38100">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -310,7 +344,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dir="5400000" dist="20000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -319,7 +353,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -328,7 +362,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -338,12 +372,12 @@
             <a:camera prst="orthographicFront">
               <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig dir="t" rig="threePt">
+            <a:lightRig rig="threePt" dir="t">
               <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
-            <a:bevelT h="25400" w="63500"/>
+            <a:bevelT w="63500" h="25400"/>
           </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
@@ -374,7 +408,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect b="180000" l="50000" r="50000" t="-80000"/>
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
           </a:path>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
@@ -393,7 +427,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect b="50000" l="50000" r="50000" t="50000"/>
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
           </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
@@ -405,20 +439,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="19.0" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="12.140625" collapsed="true"/>
+    <col min="1" max="1" width="19" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="12.109375" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
@@ -429,74 +463,74 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>7</v>
+      <c r="B3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>7</v>
+      <c r="B4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="D5" s="1"/>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="F4:G4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="F4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="4" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="6:6" x14ac:dyDescent="0.3">
       <c r="F4" t="s">
         <v>0</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>